<commit_message>
Some model updates for new classes that are being created in CV_update branch.
</commit_message>
<xml_diff>
--- a/data/Sections.xlsx
+++ b/data/Sections.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
   <si>
     <t>papers</t>
   </si>
@@ -97,9 +97,6 @@
     <t>stories</t>
   </si>
   <si>
-    <t>random</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
@@ -299,9 +296,6 @@
   </si>
   <si>
     <t>Short Stories</t>
-  </si>
-  <si>
-    <t>Random Hobbies</t>
   </si>
   <si>
     <t>about, education, jobs, awards</t>
@@ -667,30 +661,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -699,13 +693,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -713,13 +707,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -727,13 +721,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -741,13 +735,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -755,13 +749,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -775,26 +769,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDDF32E-3088-40FE-857C-01CAFCB58ABE}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -805,22 +799,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -831,16 +825,16 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -851,13 +845,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -868,13 +862,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -885,16 +879,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
         <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -905,13 +899,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -922,10 +916,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -936,13 +930,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -953,10 +947,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -967,13 +961,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -987,13 +981,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1004,16 +998,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
         <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
       </c>
       <c r="G13" s="2"/>
     </row>
@@ -1025,16 +1019,16 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1045,16 +1039,16 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1065,16 +1059,16 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1085,10 +1079,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1099,10 +1093,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1113,16 +1107,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1133,13 +1127,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1150,13 +1144,13 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1167,13 +1161,13 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1184,16 +1178,16 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1204,13 +1198,13 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1221,30 +1215,16 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Huge update of cvutils. New meta classes for handling CV and Sections
- New classes Section and CurriculumVitae
- Implemented fetch there
- Understood a lot of how classes and imports work
- Should be ready for next step into webpage model
- Also, take a look at toimplement file. Many improvements!
</commit_message>
<xml_diff>
--- a/data/Sections.xlsx
+++ b/data/Sections.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SectionManager" sheetId="1" r:id="rId1"/>
-    <sheet name="SubsectionManager" sheetId="2" r:id="rId2"/>
+    <sheet name="General" sheetId="3" r:id="rId1"/>
+    <sheet name="SectionManager" sheetId="2" r:id="rId2"/>
+    <sheet name="SecListManager" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
   <si>
     <t>papers</t>
   </si>
@@ -190,9 +191,6 @@
     <t>subsections</t>
   </si>
   <si>
-    <t>Subsection Name</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -202,9 +200,6 @@
     <t>_class</t>
   </si>
   <si>
-    <t>tag_filters</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -244,9 +239,6 @@
     <t>promotion</t>
   </si>
   <si>
-    <t>Subsection Caption</t>
-  </si>
-  <si>
     <t>Awards</t>
   </si>
   <si>
@@ -262,24 +254,15 @@
     <t>Math Contests</t>
   </si>
   <si>
-    <t>Python Projects</t>
-  </si>
-  <si>
     <t>Talks and Slides</t>
   </si>
   <si>
-    <t>Web Projects</t>
-  </si>
-  <si>
     <t>About Me</t>
   </si>
   <si>
     <t>Not Found</t>
   </si>
   <si>
-    <t>Data Science Projects</t>
-  </si>
-  <si>
     <t>All Projects</t>
   </si>
   <si>
@@ -320,13 +303,37 @@
   </si>
   <si>
     <t>given</t>
+  </si>
+  <si>
+    <t>Data Science</t>
+  </si>
+  <si>
+    <t>Web Development</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>filter_tags</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Leonardo Ignacio Martínez Sandoval</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Name of list of Sections</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,6 +343,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -363,10 +378,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,124 +662,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1A3830-3B6B-4797-9F58-D12BB526DB28}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="4" width="16" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>96</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="F3:F26">
-    <sortCondition ref="F3"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -772,7 +699,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,10 +709,10 @@
         <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>27</v>
@@ -802,19 +729,19 @@
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -825,13 +752,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>29</v>
@@ -845,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>25</v>
@@ -862,7 +789,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -879,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
@@ -981,7 +908,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
         <v>25</v>
@@ -998,7 +925,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -1009,7 +936,7 @@
       <c r="F13" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1019,7 +946,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
@@ -1028,7 +955,7 @@
         <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1048,7 +975,7 @@
         <v>47</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1059,7 +986,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -1068,7 +995,7 @@
         <v>43</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1079,7 +1006,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
@@ -1093,7 +1020,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -1107,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
@@ -1127,7 +1054,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
@@ -1144,7 +1071,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -1161,7 +1088,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D22" t="s">
         <v>25</v>
@@ -1178,13 +1105,13 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F23" t="s">
         <v>28</v>
@@ -1198,7 +1125,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
         <v>25</v>
@@ -1215,7 +1142,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1231,4 +1158,127 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="4" width="16" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="F3:F26">
+    <sortCondition ref="F3"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>